<commit_message>
allow new annotator automatically generate new type system xml even if the type system is the same
</commit_message>
<xml_diff>
--- a/conf/smoke3/smoke_context.xlsx
+++ b/conf/smoke3/smoke_context.xlsx
@@ -3938,8 +3938,8 @@
   </sheetPr>
   <dimension ref="A1:F1722"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1692" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1723" activeCellId="0" sqref="A1723"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32791,8 +32791,8 @@
   </sheetPr>
   <dimension ref="A1:F1701"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>